<commit_message>
testcase updates, munor update to SNSP calculation
</commit_message>
<xml_diff>
--- a/illustrative_testcase.xlsx
+++ b/illustrative_testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76F7A016-8255-4065-B363-B87A518E660B}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAAEFE04-AFD9-4703-8247-CB2378BE527C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">branch!$A$1:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">generator!$A$1:$R$9</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">ts_PD!$F$16:$G$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">generator!$A$1:$R$7</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">ts_PD!$F$10:$G$10</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">ts_PD!$E$19</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">ts_PD!$E$13</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
@@ -46,7 +46,7 @@
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">ts_PD!$E$18</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">ts_PD!$E$12</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -275,24 +275,12 @@
     <t>W1.2</t>
   </si>
   <si>
-    <t>W1.3</t>
-  </si>
-  <si>
-    <t>W1.4</t>
-  </si>
-  <si>
     <t>W2.1</t>
   </si>
   <si>
     <t>W2.2</t>
   </si>
   <si>
-    <t>W2.3</t>
-  </si>
-  <si>
-    <t>W2.4</t>
-  </si>
-  <si>
     <t>Bus 1</t>
   </si>
   <si>
@@ -324,24 +312,6 @@
   </si>
   <si>
     <t>t-6</t>
-  </si>
-  <si>
-    <t>t-7</t>
-  </si>
-  <si>
-    <t>t-8</t>
-  </si>
-  <si>
-    <t>t-9</t>
-  </si>
-  <si>
-    <t>t-10</t>
-  </si>
-  <si>
-    <t>t-11</t>
-  </si>
-  <si>
-    <t>t-12</t>
   </si>
   <si>
     <t>Pro-Rata</t>
@@ -464,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -526,6 +496,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -926,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -940,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -954,15 +925,15 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -970,10 +941,10 @@
         <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>48</v>
@@ -990,22 +961,10 @@
       <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
@@ -1031,22 +990,10 @@
       <c r="I2" s="9">
         <v>0</v>
       </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9">
         <v>6</v>
@@ -1072,22 +1019,10 @@
       <c r="I3" s="9">
         <v>0</v>
       </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="9">
         <v>7</v>
@@ -1113,22 +1048,10 @@
       <c r="I4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="9">
         <v>8</v>
@@ -1154,22 +1077,10 @@
       <c r="I5" s="9">
         <v>0</v>
       </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="9">
         <v>9</v>
@@ -1195,22 +1106,10 @@
       <c r="I6" s="9">
         <v>0</v>
       </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9">
-        <v>0</v>
-      </c>
-      <c r="M6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="9">
         <v>10</v>
@@ -1234,264 +1133,6 @@
         <v>0</v>
       </c>
       <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="9">
-        <v>11</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="9">
-        <v>12</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="9">
-        <v>13</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="9">
-        <v>14</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="9">
-        <v>15</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="9">
-        <v>16</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
-        <v>0</v>
-      </c>
-      <c r="M13" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1505,15 +1146,15 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J25:J26"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -1521,10 +1162,10 @@
         <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>48</v>
@@ -1541,22 +1182,10 @@
       <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9">
         <v>50</v>
@@ -1568,7 +1197,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
@@ -1582,22 +1211,10 @@
       <c r="I2" s="9">
         <v>0</v>
       </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9">
         <v>50</v>
@@ -1609,7 +1226,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F3" s="9">
         <v>0</v>
@@ -1623,22 +1240,10 @@
       <c r="I3" s="9">
         <v>0</v>
       </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="9">
         <v>50</v>
@@ -1650,7 +1255,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F4" s="9">
         <v>0</v>
@@ -1664,22 +1269,10 @@
       <c r="I4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="9">
         <v>50</v>
@@ -1691,7 +1284,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F5" s="9">
         <v>0</v>
@@ -1705,22 +1298,10 @@
       <c r="I5" s="9">
         <v>0</v>
       </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="9">
         <v>50</v>
@@ -1732,7 +1313,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F6" s="9">
         <v>0</v>
@@ -1746,22 +1327,10 @@
       <c r="I6" s="9">
         <v>0</v>
       </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9">
-        <v>0</v>
-      </c>
-      <c r="M6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="9">
         <v>50</v>
@@ -1773,7 +1342,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F7" s="9">
         <v>0</v>
@@ -1785,264 +1354,6 @@
         <v>0</v>
       </c>
       <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="9">
-        <v>50</v>
-      </c>
-      <c r="C8" s="9">
-        <v>50</v>
-      </c>
-      <c r="D8" s="9">
-        <v>50</v>
-      </c>
-      <c r="E8" s="9">
-        <v>80</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="9">
-        <v>50</v>
-      </c>
-      <c r="C9" s="9">
-        <v>50</v>
-      </c>
-      <c r="D9" s="9">
-        <v>50</v>
-      </c>
-      <c r="E9" s="9">
-        <v>80</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="9">
-        <v>50</v>
-      </c>
-      <c r="C10" s="9">
-        <v>50</v>
-      </c>
-      <c r="D10" s="9">
-        <v>50</v>
-      </c>
-      <c r="E10" s="9">
-        <v>80</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="9">
-        <v>50</v>
-      </c>
-      <c r="C11" s="9">
-        <v>50</v>
-      </c>
-      <c r="D11" s="9">
-        <v>50</v>
-      </c>
-      <c r="E11" s="9">
-        <v>80</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="9">
-        <v>50</v>
-      </c>
-      <c r="C12" s="9">
-        <v>50</v>
-      </c>
-      <c r="D12" s="9">
-        <v>50</v>
-      </c>
-      <c r="E12" s="9">
-        <v>80</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="9">
-        <v>50</v>
-      </c>
-      <c r="C13" s="9">
-        <v>50</v>
-      </c>
-      <c r="D13" s="9">
-        <v>50</v>
-      </c>
-      <c r="E13" s="9">
-        <v>80</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
-        <v>0</v>
-      </c>
-      <c r="M13" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2056,15 +1367,15 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -2072,10 +1383,10 @@
         <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>48</v>
@@ -2092,22 +1403,10 @@
       <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10">
         <v>100</v>
@@ -2119,36 +1418,24 @@
         <v>100</v>
       </c>
       <c r="E2" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F2" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G2" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H2" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I2" s="20">
-        <v>30</v>
-      </c>
-      <c r="J2" s="20">
-        <v>30</v>
-      </c>
-      <c r="K2" s="20">
-        <v>30</v>
-      </c>
-      <c r="L2" s="20">
-        <v>30</v>
-      </c>
-      <c r="M2" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10">
         <v>100</v>
@@ -2160,36 +1447,24 @@
         <v>100</v>
       </c>
       <c r="E3" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F3" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G3" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H3" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I3" s="20">
-        <v>30</v>
-      </c>
-      <c r="J3" s="20">
-        <v>30</v>
-      </c>
-      <c r="K3" s="20">
-        <v>30</v>
-      </c>
-      <c r="L3" s="20">
-        <v>30</v>
-      </c>
-      <c r="M3" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="10">
         <v>100</v>
@@ -2201,36 +1476,24 @@
         <v>100</v>
       </c>
       <c r="E4" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F4" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G4" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H4" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I4" s="20">
-        <v>30</v>
-      </c>
-      <c r="J4" s="20">
-        <v>30</v>
-      </c>
-      <c r="K4" s="20">
-        <v>30</v>
-      </c>
-      <c r="L4" s="20">
-        <v>30</v>
-      </c>
-      <c r="M4" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10">
         <v>100</v>
@@ -2242,36 +1505,24 @@
         <v>100</v>
       </c>
       <c r="E5" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F5" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G5" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="H5" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="I5" s="20">
-        <v>5</v>
-      </c>
-      <c r="J5" s="20">
-        <v>30</v>
-      </c>
-      <c r="K5" s="20">
-        <v>30</v>
-      </c>
-      <c r="L5" s="20">
-        <v>30</v>
-      </c>
-      <c r="M5" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="10">
         <v>100</v>
@@ -2283,36 +1534,24 @@
         <v>100</v>
       </c>
       <c r="E6" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F6" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G6" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H6" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I6" s="20">
-        <v>30</v>
-      </c>
-      <c r="J6" s="20">
-        <v>5</v>
-      </c>
-      <c r="K6" s="20">
-        <v>5</v>
-      </c>
-      <c r="L6" s="20">
-        <v>5</v>
-      </c>
-      <c r="M6" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="10">
         <v>100</v>
@@ -2324,277 +1563,19 @@
         <v>100</v>
       </c>
       <c r="E7" s="10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F7" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G7" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="H7" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="I7" s="20">
-        <v>5</v>
-      </c>
-      <c r="J7" s="20">
-        <v>5</v>
-      </c>
-      <c r="K7" s="20">
-        <v>5</v>
-      </c>
-      <c r="L7" s="20">
-        <v>5</v>
-      </c>
-      <c r="M7" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="10">
-        <v>100</v>
-      </c>
-      <c r="C8" s="10">
-        <v>100</v>
-      </c>
-      <c r="D8" s="10">
-        <v>100</v>
-      </c>
-      <c r="E8" s="10">
-        <v>200</v>
-      </c>
-      <c r="F8" s="20">
-        <v>30</v>
-      </c>
-      <c r="G8" s="20">
-        <v>30</v>
-      </c>
-      <c r="H8" s="20">
-        <v>30</v>
-      </c>
-      <c r="I8" s="20">
-        <v>30</v>
-      </c>
-      <c r="J8" s="20">
-        <v>30</v>
-      </c>
-      <c r="K8" s="20">
-        <v>30</v>
-      </c>
-      <c r="L8" s="20">
-        <v>30</v>
-      </c>
-      <c r="M8" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="10">
-        <v>100</v>
-      </c>
-      <c r="C9" s="10">
-        <v>100</v>
-      </c>
-      <c r="D9" s="10">
-        <v>100</v>
-      </c>
-      <c r="E9" s="10">
-        <v>200</v>
-      </c>
-      <c r="F9" s="20">
-        <v>30</v>
-      </c>
-      <c r="G9" s="20">
-        <v>30</v>
-      </c>
-      <c r="H9" s="20">
-        <v>30</v>
-      </c>
-      <c r="I9" s="20">
-        <v>30</v>
-      </c>
-      <c r="J9" s="20">
-        <v>30</v>
-      </c>
-      <c r="K9" s="20">
-        <v>30</v>
-      </c>
-      <c r="L9" s="20">
-        <v>30</v>
-      </c>
-      <c r="M9" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="10">
-        <v>100</v>
-      </c>
-      <c r="C10" s="10">
-        <v>100</v>
-      </c>
-      <c r="D10" s="10">
-        <v>100</v>
-      </c>
-      <c r="E10" s="10">
-        <v>200</v>
-      </c>
-      <c r="F10" s="20">
-        <v>30</v>
-      </c>
-      <c r="G10" s="20">
-        <v>30</v>
-      </c>
-      <c r="H10" s="20">
-        <v>30</v>
-      </c>
-      <c r="I10" s="20">
-        <v>30</v>
-      </c>
-      <c r="J10" s="20">
-        <v>30</v>
-      </c>
-      <c r="K10" s="20">
-        <v>30</v>
-      </c>
-      <c r="L10" s="20">
-        <v>30</v>
-      </c>
-      <c r="M10" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="10">
-        <v>100</v>
-      </c>
-      <c r="C11" s="10">
-        <v>100</v>
-      </c>
-      <c r="D11" s="10">
-        <v>100</v>
-      </c>
-      <c r="E11" s="10">
-        <v>200</v>
-      </c>
-      <c r="F11" s="20">
-        <v>5</v>
-      </c>
-      <c r="G11" s="20">
-        <v>5</v>
-      </c>
-      <c r="H11" s="20">
-        <v>5</v>
-      </c>
-      <c r="I11" s="20">
-        <v>5</v>
-      </c>
-      <c r="J11" s="20">
-        <v>30</v>
-      </c>
-      <c r="K11" s="20">
-        <v>30</v>
-      </c>
-      <c r="L11" s="20">
-        <v>30</v>
-      </c>
-      <c r="M11" s="20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="10">
-        <v>100</v>
-      </c>
-      <c r="C12" s="10">
-        <v>100</v>
-      </c>
-      <c r="D12" s="10">
-        <v>100</v>
-      </c>
-      <c r="E12" s="10">
-        <v>200</v>
-      </c>
-      <c r="F12" s="20">
-        <v>30</v>
-      </c>
-      <c r="G12" s="20">
-        <v>30</v>
-      </c>
-      <c r="H12" s="20">
-        <v>30</v>
-      </c>
-      <c r="I12" s="20">
-        <v>30</v>
-      </c>
-      <c r="J12" s="20">
-        <v>5</v>
-      </c>
-      <c r="K12" s="20">
-        <v>5</v>
-      </c>
-      <c r="L12" s="20">
-        <v>5</v>
-      </c>
-      <c r="M12" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="10">
-        <v>100</v>
-      </c>
-      <c r="C13" s="10">
-        <v>100</v>
-      </c>
-      <c r="D13" s="10">
-        <v>100</v>
-      </c>
-      <c r="E13" s="10">
-        <v>200</v>
-      </c>
-      <c r="F13" s="20">
-        <v>5</v>
-      </c>
-      <c r="G13" s="20">
-        <v>5</v>
-      </c>
-      <c r="H13" s="20">
-        <v>5</v>
-      </c>
-      <c r="I13" s="20">
-        <v>5</v>
-      </c>
-      <c r="J13" s="20">
-        <v>5</v>
-      </c>
-      <c r="K13" s="20">
-        <v>5</v>
-      </c>
-      <c r="L13" s="20">
-        <v>5</v>
-      </c>
-      <c r="M13" s="20">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2607,15 +1588,15 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:M3"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -2623,10 +1604,10 @@
         <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>48</v>
@@ -2643,22 +1624,10 @@
       <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10">
         <v>40</v>
@@ -2684,22 +1653,10 @@
       <c r="I2" s="10">
         <v>80</v>
       </c>
-      <c r="J2" s="10">
-        <v>80</v>
-      </c>
-      <c r="K2" s="10">
-        <v>80</v>
-      </c>
-      <c r="L2" s="10">
-        <v>80</v>
-      </c>
-      <c r="M2" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10">
         <v>40</v>
@@ -2725,22 +1682,10 @@
       <c r="I3" s="10">
         <v>80</v>
       </c>
-      <c r="J3" s="10">
-        <v>80</v>
-      </c>
-      <c r="K3" s="10">
-        <v>80</v>
-      </c>
-      <c r="L3" s="10">
-        <v>80</v>
-      </c>
-      <c r="M3" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="10">
         <v>40</v>
@@ -2766,22 +1711,10 @@
       <c r="I4" s="10">
         <v>80</v>
       </c>
-      <c r="J4" s="10">
-        <v>80</v>
-      </c>
-      <c r="K4" s="10">
-        <v>80</v>
-      </c>
-      <c r="L4" s="10">
-        <v>80</v>
-      </c>
-      <c r="M4" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10">
         <v>40</v>
@@ -2807,22 +1740,10 @@
       <c r="I5" s="10">
         <v>80</v>
       </c>
-      <c r="J5" s="10">
-        <v>80</v>
-      </c>
-      <c r="K5" s="10">
-        <v>80</v>
-      </c>
-      <c r="L5" s="10">
-        <v>80</v>
-      </c>
-      <c r="M5" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="10">
         <v>40</v>
@@ -2848,22 +1769,10 @@
       <c r="I6" s="10">
         <v>80</v>
       </c>
-      <c r="J6" s="10">
-        <v>80</v>
-      </c>
-      <c r="K6" s="10">
-        <v>80</v>
-      </c>
-      <c r="L6" s="10">
-        <v>80</v>
-      </c>
-      <c r="M6" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="10">
         <v>40</v>
@@ -2887,264 +1796,6 @@
         <v>80</v>
       </c>
       <c r="I7" s="10">
-        <v>80</v>
-      </c>
-      <c r="J7" s="10">
-        <v>80</v>
-      </c>
-      <c r="K7" s="10">
-        <v>80</v>
-      </c>
-      <c r="L7" s="10">
-        <v>80</v>
-      </c>
-      <c r="M7" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="10">
-        <v>40</v>
-      </c>
-      <c r="C8" s="10">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10">
-        <v>40</v>
-      </c>
-      <c r="E8" s="10">
-        <v>40</v>
-      </c>
-      <c r="F8" s="10">
-        <v>80</v>
-      </c>
-      <c r="G8" s="10">
-        <v>80</v>
-      </c>
-      <c r="H8" s="10">
-        <v>80</v>
-      </c>
-      <c r="I8" s="10">
-        <v>80</v>
-      </c>
-      <c r="J8" s="10">
-        <v>80</v>
-      </c>
-      <c r="K8" s="10">
-        <v>80</v>
-      </c>
-      <c r="L8" s="10">
-        <v>80</v>
-      </c>
-      <c r="M8" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="10">
-        <v>40</v>
-      </c>
-      <c r="C9" s="10">
-        <v>40</v>
-      </c>
-      <c r="D9" s="10">
-        <v>40</v>
-      </c>
-      <c r="E9" s="10">
-        <v>40</v>
-      </c>
-      <c r="F9" s="10">
-        <v>80</v>
-      </c>
-      <c r="G9" s="10">
-        <v>80</v>
-      </c>
-      <c r="H9" s="10">
-        <v>80</v>
-      </c>
-      <c r="I9" s="10">
-        <v>80</v>
-      </c>
-      <c r="J9" s="10">
-        <v>80</v>
-      </c>
-      <c r="K9" s="10">
-        <v>80</v>
-      </c>
-      <c r="L9" s="10">
-        <v>80</v>
-      </c>
-      <c r="M9" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="10">
-        <v>40</v>
-      </c>
-      <c r="C10" s="10">
-        <v>40</v>
-      </c>
-      <c r="D10" s="10">
-        <v>40</v>
-      </c>
-      <c r="E10" s="10">
-        <v>40</v>
-      </c>
-      <c r="F10" s="10">
-        <v>80</v>
-      </c>
-      <c r="G10" s="10">
-        <v>80</v>
-      </c>
-      <c r="H10" s="10">
-        <v>80</v>
-      </c>
-      <c r="I10" s="10">
-        <v>80</v>
-      </c>
-      <c r="J10" s="10">
-        <v>80</v>
-      </c>
-      <c r="K10" s="10">
-        <v>80</v>
-      </c>
-      <c r="L10" s="10">
-        <v>80</v>
-      </c>
-      <c r="M10" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="10">
-        <v>40</v>
-      </c>
-      <c r="C11" s="10">
-        <v>40</v>
-      </c>
-      <c r="D11" s="10">
-        <v>40</v>
-      </c>
-      <c r="E11" s="10">
-        <v>40</v>
-      </c>
-      <c r="F11" s="10">
-        <v>80</v>
-      </c>
-      <c r="G11" s="10">
-        <v>80</v>
-      </c>
-      <c r="H11" s="10">
-        <v>80</v>
-      </c>
-      <c r="I11" s="10">
-        <v>80</v>
-      </c>
-      <c r="J11" s="10">
-        <v>80</v>
-      </c>
-      <c r="K11" s="10">
-        <v>80</v>
-      </c>
-      <c r="L11" s="10">
-        <v>80</v>
-      </c>
-      <c r="M11" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="10">
-        <v>40</v>
-      </c>
-      <c r="C12" s="10">
-        <v>40</v>
-      </c>
-      <c r="D12" s="10">
-        <v>40</v>
-      </c>
-      <c r="E12" s="10">
-        <v>40</v>
-      </c>
-      <c r="F12" s="10">
-        <v>80</v>
-      </c>
-      <c r="G12" s="10">
-        <v>80</v>
-      </c>
-      <c r="H12" s="10">
-        <v>80</v>
-      </c>
-      <c r="I12" s="10">
-        <v>80</v>
-      </c>
-      <c r="J12" s="10">
-        <v>80</v>
-      </c>
-      <c r="K12" s="10">
-        <v>80</v>
-      </c>
-      <c r="L12" s="10">
-        <v>80</v>
-      </c>
-      <c r="M12" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="10">
-        <v>40</v>
-      </c>
-      <c r="C13" s="10">
-        <v>40</v>
-      </c>
-      <c r="D13" s="10">
-        <v>40</v>
-      </c>
-      <c r="E13" s="10">
-        <v>40</v>
-      </c>
-      <c r="F13" s="10">
-        <v>80</v>
-      </c>
-      <c r="G13" s="10">
-        <v>80</v>
-      </c>
-      <c r="H13" s="10">
-        <v>80</v>
-      </c>
-      <c r="I13" s="10">
-        <v>80</v>
-      </c>
-      <c r="J13" s="10">
-        <v>80</v>
-      </c>
-      <c r="K13" s="10">
-        <v>80</v>
-      </c>
-      <c r="L13" s="10">
-        <v>80</v>
-      </c>
-      <c r="M13" s="10">
         <v>80</v>
       </c>
     </row>
@@ -3190,7 +1841,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3283,10 +1934,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3313,227 +1964,104 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="20">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C2" s="20">
-        <f>80</f>
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="D2" s="20">
-        <f>80</f>
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="20">
-        <f>80/0.75</f>
-        <v>106.66666666666667</v>
+        <v>55</v>
       </c>
       <c r="C3" s="20">
-        <f t="shared" ref="C3:D13" si="0">80/0.75</f>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="D3" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="20">
-        <f>80/0.5</f>
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="C4" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="20">
-        <f t="shared" ref="B5:B7" si="1">80/0.5</f>
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="C5" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="20">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="C6" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="20">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="C7" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
+        <v>107</v>
       </c>
       <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="20">
-        <v>80</v>
-      </c>
-      <c r="C8" s="20">
-        <f>80</f>
-        <v>80</v>
-      </c>
-      <c r="D8" s="20">
-        <f>80</f>
-        <v>80</v>
-      </c>
-      <c r="E8" s="18"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="20">
-        <f>80/0.75</f>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="C9" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="D9" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="E9" s="18"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="20">
-        <f>80/0.5</f>
-        <v>160</v>
-      </c>
-      <c r="C10" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="D10" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="20">
-        <f t="shared" ref="B11:B13" si="2">80/0.5</f>
-        <v>160</v>
-      </c>
-      <c r="C11" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="D11" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="E11" s="18"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="20">
-        <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="C12" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="D12" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="20">
-        <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="C13" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="D13" s="20">
-        <f t="shared" si="0"/>
-        <v>106.66666666666667</v>
-      </c>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F16" s="17"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="6"/>
+      <c r="G12" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3548,10 +2076,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A8" sqref="A8:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3576,7 +2104,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>7000</v>
@@ -3590,7 +2118,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
         <v>7000</v>
@@ -3604,7 +2132,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>7000</v>
@@ -3618,7 +2146,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3">
         <v>7000</v>
@@ -3632,7 +2160,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3">
         <v>7000</v>
@@ -3646,7 +2174,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3">
         <v>7000</v>
@@ -3655,90 +2183,6 @@
         <v>7000</v>
       </c>
       <c r="D7" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C8" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C11" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D11" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C12" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D12" s="3">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C13" s="3">
-        <v>7000</v>
-      </c>
-      <c r="D13" s="3">
         <v>7000</v>
       </c>
     </row>
@@ -3870,10 +2314,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C7" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3895,7 +2339,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>90</v>
@@ -3906,7 +2350,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
         <v>90</v>
@@ -3917,7 +2361,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>90</v>
@@ -3928,100 +2372,34 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3">
         <v>90</v>
       </c>
       <c r="C5" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3">
         <v>90</v>
       </c>
       <c r="C6" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3">
         <v>90</v>
       </c>
       <c r="C7" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="3">
-        <v>90</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="3">
-        <v>90</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="3">
-        <v>90</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="3">
-        <v>90</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="3">
-        <v>90</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="3">
-        <v>90</v>
-      </c>
-      <c r="C13" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4164,10 +2542,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="M21" sqref="M21:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4189,7 +2567,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>20</v>
@@ -4200,7 +2578,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
         <v>20</v>
@@ -4211,7 +2589,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>20</v>
@@ -4222,100 +2600,34 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3">
         <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="3">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="3">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="3">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="3">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="3">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="3">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4330,10 +2642,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4377,7 +2689,7 @@
         <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -4386,7 +2698,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>20</v>
@@ -4427,7 +2739,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -4443,7 +2755,7 @@
         <v>100</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>36</v>
@@ -4466,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>39</v>
@@ -4475,7 +2787,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -4491,7 +2803,7 @@
         <v>100</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>36</v>
@@ -4514,7 +2826,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>39</v>
@@ -4523,7 +2835,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H4" s="10">
         <v>1</v>
@@ -4539,7 +2851,7 @@
         <v>100</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>36</v>
@@ -4571,7 +2883,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H5" s="10">
         <v>1</v>
@@ -4587,7 +2899,7 @@
         <v>200</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>36</v>
@@ -4613,7 +2925,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -4622,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10">
@@ -4636,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="20">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>28</v>
@@ -4665,16 +2977,16 @@
         <v>50</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10">
@@ -4688,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="20">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>28</v>
@@ -4711,22 +3023,22 @@
     </row>
     <row r="8" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="9">
-        <v>3</v>
-      </c>
       <c r="F8" s="10" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10">
@@ -4740,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="20">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>28</v>
@@ -4763,22 +3075,22 @@
     </row>
     <row r="9" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10">
@@ -4792,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="20">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>28</v>
@@ -4813,229 +3125,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12">
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="20">
-        <v>20</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="10">
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="13">
-        <v>1000</v>
-      </c>
-      <c r="R10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <v>2</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2</v>
-      </c>
-      <c r="E11" s="9">
-        <v>2</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10">
-        <v>1</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="20">
-        <v>20</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="10">
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="13">
-        <v>1000</v>
-      </c>
-      <c r="R11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2</v>
-      </c>
-      <c r="E12" s="9">
-        <v>3</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="20">
-        <v>20</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="10">
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="13">
-        <v>1000</v>
-      </c>
-      <c r="R12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
-        <v>2</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="9">
-        <v>2</v>
-      </c>
-      <c r="E13" s="9">
-        <v>4</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10">
-        <v>1</v>
-      </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="20">
-        <v>20</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="10">
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="13">
-        <v>1000</v>
-      </c>
-      <c r="R13" s="22">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:R9" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
+  <autoFilter ref="A1:R7" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E13">
+  <conditionalFormatting sqref="D2:E9">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>($C2&lt;&gt;"LIFO")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F13">
+  <conditionalFormatting sqref="F2:F9">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>($C2&lt;&gt;"Pro-Rata")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13" xr:uid="{93378767-7322-405A-9798-43C52CE33CE3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{93378767-7322-405A-9798-43C52CE33CE3}">
       <formula1>"Individual,Uncontrollable,LIFO,Pro-Rata"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5045,26 +3149,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
     <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
@@ -5293,7 +3377,46 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5301,7 +3424,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5318,23 +3441,4 @@
     <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>